<commit_message>
javdb support Amateur & Censored in the same time
</commit_message>
<xml_diff>
--- a/javsdt/【特征对照表】.xlsx
+++ b/javsdt/【特征对照表】.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4121" uniqueCount="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4124" uniqueCount="1354">
   <si>
     <t>原简体特征</t>
   </si>
@@ -4088,9 +4088,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -4102,35 +4102,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -4138,32 +4109,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4199,9 +4147,67 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4223,25 +4229,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4254,7 +4254,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4266,31 +4362,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4302,37 +4410,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4350,91 +4428,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4445,6 +4445,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -4472,6 +4492,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -4482,6 +4511,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -4501,60 +4545,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4563,133 +4563,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5050,7 +5050,7 @@
   <dimension ref="A1:D326"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
-      <selection activeCell="A326" sqref="A326"/>
+      <selection activeCell="M325" sqref="M325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -8634,7 +8634,7 @@
       </c>
     </row>
     <row r="326" spans="1:3">
-      <c r="A326" s="2" t="s">
+      <c r="A326" s="1" t="s">
         <v>571</v>
       </c>
       <c r="B326" s="1" t="s">
@@ -17348,10 +17348,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D261"/>
+  <dimension ref="A1:D262"/>
   <sheetViews>
     <sheetView topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="B266" sqref="B266"/>
+      <selection activeCell="G267" sqref="G267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -20230,6 +20230,17 @@
         <v>269</v>
       </c>
     </row>
+    <row r="262" spans="1:3">
+      <c r="A262" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>